<commit_message>
cleaned up some player names
</commit_message>
<xml_diff>
--- a/_site/data/2022Winter_DraftedTeams_Emails_Website.xlsx
+++ b/_site/data/2022Winter_DraftedTeams_Emails_Website.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pdwalker\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EFBFD9-6173-49B9-A16C-84883B6EC327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2EFBBB-ED01-4081-A09E-8A3344A7FAB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="975" windowWidth="25575" windowHeight="14415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31155" yWindow="435" windowWidth="25575" windowHeight="14415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="329">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1009,6 +1009,9 @@
   </si>
   <si>
     <t>XXL</t>
+  </si>
+  <si>
+    <t>Carolyn Godwin</t>
   </si>
 </sst>
 </file>
@@ -1104,7 +1107,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1118,7 +1121,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
@@ -5273,13 +5275,14 @@
   <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.625" customWidth="1"/>
     <col min="2" max="2" width="22.125" customWidth="1"/>
+    <col min="3" max="3" width="41.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.625" customWidth="1"/>
     <col min="6" max="6" width="25.25" customWidth="1"/>
     <col min="7" max="7" width="7.625" customWidth="1"/>
@@ -5301,10 +5304,10 @@
       <c r="E1" s="11" t="s">
         <v>322</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>323</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>324</v>
       </c>
     </row>
@@ -5321,7 +5324,7 @@
       <c r="D2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
         <v>325</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -5344,7 +5347,7 @@
       <c r="D3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="15" t="s">
         <v>325</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -5356,117 +5359,117 @@
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>111</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>116</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>116</v>
+        <v>14</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>325</v>
+      <c r="E4" s="16" t="s">
+        <v>326</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>115</v>
+        <v>13</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>111</v>
+        <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>150</v>
+        <v>24</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>150</v>
+        <v>24</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>149</v>
+        <v>23</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>228</v>
+        <v>36</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>228</v>
+        <v>36</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>227</v>
+        <v>35</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>249</v>
+        <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>248</v>
+        <v>39</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>248</v>
+        <v>39</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>247</v>
+        <v>38</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>249</v>
+        <v>15</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>265</v>
+        <v>45</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>265</v>
+        <v>45</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>46</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>264</v>
+        <v>44</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -5474,22 +5477,22 @@
         <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -5497,22 +5500,22 @@
         <v>15</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -5520,22 +5523,22 @@
         <v>15</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -5543,22 +5546,22 @@
         <v>15</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -5566,22 +5569,22 @@
         <v>15</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -5589,22 +5592,22 @@
         <v>15</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -5612,22 +5615,22 @@
         <v>15</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -5635,22 +5638,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -5658,22 +5661,22 @@
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -5681,22 +5684,22 @@
         <v>15</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>68</v>
+        <v>97</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -5704,22 +5707,22 @@
         <v>15</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -5727,177 +5730,177 @@
         <v>15</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="17" t="s">
+      <c r="B21" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="16" t="s">
         <v>326</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>15</v>
+        <v>111</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>326</v>
+        <v>17</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>325</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>15</v>
+        <v>111</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>98</v>
+        <v>150</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>98</v>
+        <v>150</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="17" t="s">
-        <v>326</v>
+      <c r="E23" s="15" t="s">
+        <v>325</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>97</v>
+        <v>149</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>15</v>
+        <v>111</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>15</v>
+        <v>111</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" s="17" t="s">
+      <c r="A26" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="16" t="s">
         <v>326</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>110</v>
+      <c r="B27" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>328</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="17" t="s">
+      <c r="E27" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -5905,19 +5908,19 @@
         <v>111</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E28" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>40</v>
@@ -5928,19 +5931,19 @@
         <v>111</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E29" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>16</v>
@@ -5950,23 +5953,23 @@
       <c r="A30" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>125</v>
+      <c r="B30" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>137</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -5974,19 +5977,19 @@
         <v>111</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>40</v>
@@ -5997,19 +6000,19 @@
         <v>111</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="17" t="s">
+      <c r="E32" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>16</v>
@@ -6020,19 +6023,19 @@
         <v>111</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E33" s="17" t="s">
+      <c r="E33" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>40</v>
@@ -6042,23 +6045,23 @@
       <c r="A34" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>141</v>
+      <c r="B34" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>156</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E34" s="17" t="s">
+      <c r="E34" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -6066,22 +6069,22 @@
         <v>111</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E35" s="17" t="s">
+      <c r="E35" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -6089,19 +6092,19 @@
         <v>111</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E36" s="17" t="s">
+      <c r="E36" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>40</v>
@@ -6111,23 +6114,23 @@
       <c r="A37" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>156</v>
+      <c r="B37" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>166</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E37" s="17" t="s">
+      <c r="E37" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -6135,19 +6138,19 @@
         <v>111</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E38" s="17" t="s">
+      <c r="E38" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>40</v>
@@ -6158,22 +6161,22 @@
         <v>111</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E39" s="17" t="s">
+      <c r="E39" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -6181,65 +6184,65 @@
         <v>111</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E40" s="17" t="s">
+      <c r="E40" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>111</v>
+        <v>16</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>168</v>
+        <v>228</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>168</v>
+        <v>228</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E41" s="17" t="s">
-        <v>326</v>
+      <c r="E41" s="15" t="s">
+        <v>325</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>167</v>
+        <v>227</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>111</v>
+        <v>16</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E42" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>37</v>
@@ -6247,25 +6250,25 @@
     </row>
     <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>111</v>
+        <v>16</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E43" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -6273,19 +6276,19 @@
         <v>16</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E44" s="17" t="s">
+      <c r="E44" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>37</v>
@@ -6296,22 +6299,22 @@
         <v>16</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E45" s="17" t="s">
+      <c r="E45" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -6319,22 +6322,22 @@
         <v>16</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E46" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E46" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -6342,22 +6345,22 @@
         <v>16</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E47" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E47" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -6365,19 +6368,19 @@
         <v>16</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E48" s="17" t="s">
+      <c r="E48" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>16</v>
@@ -6388,22 +6391,22 @@
         <v>16</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E49" s="17" t="s">
+      <c r="E49" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -6411,19 +6414,19 @@
         <v>16</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E50" s="17" t="s">
+      <c r="E50" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>16</v>
@@ -6434,22 +6437,22 @@
         <v>16</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E51" s="17" t="s">
+      <c r="E51" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -6457,22 +6460,22 @@
         <v>16</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E52" s="17" t="s">
+      <c r="E52" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -6480,22 +6483,22 @@
         <v>16</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E53" s="17" t="s">
+      <c r="E53" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -6503,22 +6506,22 @@
         <v>16</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E54" s="17" t="s">
+      <c r="E54" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -6526,19 +6529,19 @@
         <v>16</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E55" s="17" t="s">
+      <c r="E55" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>16</v>
@@ -6549,22 +6552,22 @@
         <v>16</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E56" s="17" t="s">
+      <c r="E56" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -6572,22 +6575,22 @@
         <v>16</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E57" s="17" t="s">
+      <c r="E57" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -6595,68 +6598,68 @@
         <v>16</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E58" s="17" t="s">
+      <c r="E58" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>16</v>
+        <v>249</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E59" s="17" t="s">
-        <v>326</v>
+        <v>17</v>
+      </c>
+      <c r="E59" s="15" t="s">
+        <v>325</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>16</v>
+        <v>249</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E60" s="17" t="s">
-        <v>326</v>
+      <c r="E60" s="15" t="s">
+        <v>325</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -6672,7 +6675,7 @@
       <c r="D61" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E61" s="17" t="s">
+      <c r="E61" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F61" s="4" t="s">
@@ -6695,7 +6698,7 @@
       <c r="D62" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E62" s="17" t="s">
+      <c r="E62" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F62" s="4" t="s">
@@ -6718,7 +6721,7 @@
       <c r="D63" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E63" s="17" t="s">
+      <c r="E63" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F63" s="4" t="s">
@@ -6741,7 +6744,7 @@
       <c r="D64" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E64" s="17" t="s">
+      <c r="E64" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F64" s="4" t="s">
@@ -6764,7 +6767,7 @@
       <c r="D65" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E65" s="17" t="s">
+      <c r="E65" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F65" s="4" t="s">
@@ -6787,7 +6790,7 @@
       <c r="D66" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E66" s="17" t="s">
+      <c r="E66" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F66" s="4" t="s">
@@ -6810,7 +6813,7 @@
       <c r="D67" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E67" s="17" t="s">
+      <c r="E67" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F67" s="4" t="s">
@@ -6833,7 +6836,7 @@
       <c r="D68" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E68" s="17" t="s">
+      <c r="E68" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F68" s="4" t="s">
@@ -6856,7 +6859,7 @@
       <c r="D69" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E69" s="17" t="s">
+      <c r="E69" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F69" s="4" t="s">
@@ -6879,7 +6882,7 @@
       <c r="D70" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E70" s="17" t="s">
+      <c r="E70" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F70" s="4" t="s">
@@ -6902,7 +6905,7 @@
       <c r="D71" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E71" s="17" t="s">
+      <c r="E71" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F71" s="4" t="s">
@@ -6925,7 +6928,7 @@
       <c r="D72" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E72" s="17" t="s">
+      <c r="E72" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F72" s="4" t="s">
@@ -6948,7 +6951,7 @@
       <c r="D73" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E73" s="17" t="s">
+      <c r="E73" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F73" s="4" t="s">
@@ -6971,7 +6974,7 @@
       <c r="D74" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E74" s="17" t="s">
+      <c r="E74" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F74" s="4" t="s">
@@ -6994,7 +6997,7 @@
       <c r="D75" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E75" s="17" t="s">
+      <c r="E75" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F75" s="4" t="s">
@@ -7017,7 +7020,7 @@
       <c r="D76" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E76" s="17" t="s">
+      <c r="E76" s="16" t="s">
         <v>326</v>
       </c>
       <c r="F76" s="4" t="s">
@@ -7030,7 +7033,8 @@
   </sheetData>
   <autoFilter ref="A1:G76" xr:uid="{F2BD999F-A439-411E-8987-30909891D5D5}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G76">
-      <sortCondition ref="E1:E76"/>
+      <sortCondition ref="A2:A76"/>
+      <sortCondition ref="E2:E76"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="A1:A999">

</xml_diff>

<commit_message>
updated winter with schedule and logo
</commit_message>
<xml_diff>
--- a/_site/data/2022Winter_DraftedTeams_Emails_Website.xlsx
+++ b/_site/data/2022Winter_DraftedTeams_Emails_Website.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pdwalker\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2EFBBB-ED01-4081-A09E-8A3344A7FAB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C03FEFD-ED2E-4F10-97AC-A40EF489A426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31155" yWindow="435" windowWidth="25575" windowHeight="14415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2700" yWindow="630" windowWidth="25575" windowHeight="14760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="gamesched" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$G$76</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="345">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1012,12 +1013,63 @@
   </si>
   <si>
     <t>Carolyn Godwin</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
+  <si>
+    <t>Field 1</t>
+  </si>
+  <si>
+    <t>Field 2</t>
+  </si>
+  <si>
+    <t>Counts</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>M vs PM</t>
+  </si>
+  <si>
+    <t>JL vs SC</t>
+  </si>
+  <si>
+    <t>Regular</t>
+  </si>
+  <si>
+    <t>M vs JL</t>
+  </si>
+  <si>
+    <t>PM vs SC</t>
+  </si>
+  <si>
+    <t>M vs SC</t>
+  </si>
+  <si>
+    <t>PM vs JL</t>
+  </si>
+  <si>
+    <t>Tourney</t>
+  </si>
+  <si>
+    <t>TBD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mmm\ d"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1107,7 +1159,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1125,6 +1177,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5274,7 +5330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2BD999F-A439-411E-8987-30909891D5D5}">
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -7059,4 +7115,515 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC042FE7-DD2C-4227-BB73-8C720EB7799C}">
+  <dimension ref="A1:L20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:L20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>332</v>
+      </c>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>333</v>
+      </c>
+      <c r="I1" s="17"/>
+      <c r="J1" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>334</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="18">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18">
+        <v>1</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="H2" s="19">
+        <v>6</v>
+      </c>
+      <c r="I2" s="17"/>
+      <c r="J2" s="18">
+        <v>1</v>
+      </c>
+      <c r="K2" s="20">
+        <v>44569</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="18">
+        <v>1</v>
+      </c>
+      <c r="B3" s="18">
+        <v>2</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="H3" s="19">
+        <v>5</v>
+      </c>
+      <c r="I3" s="17"/>
+      <c r="J3" s="18">
+        <v>2</v>
+      </c>
+      <c r="K3" s="20">
+        <v>44576</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="18">
+        <v>2</v>
+      </c>
+      <c r="B4" s="18">
+        <v>1</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="H4" s="19">
+        <v>5</v>
+      </c>
+      <c r="I4" s="17"/>
+      <c r="J4" s="18">
+        <v>3</v>
+      </c>
+      <c r="K4" s="20">
+        <v>44583</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="18">
+        <v>2</v>
+      </c>
+      <c r="B5" s="18">
+        <v>2</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="H5" s="19">
+        <v>6</v>
+      </c>
+      <c r="I5" s="17"/>
+      <c r="J5" s="18">
+        <v>4</v>
+      </c>
+      <c r="K5" s="20">
+        <v>44590</v>
+      </c>
+      <c r="L5" s="18" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="18">
+        <v>3</v>
+      </c>
+      <c r="B6" s="18">
+        <v>1</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="H6" s="19">
+        <v>5</v>
+      </c>
+      <c r="I6" s="17"/>
+      <c r="J6" s="18">
+        <v>5</v>
+      </c>
+      <c r="K6" s="20">
+        <v>44597</v>
+      </c>
+      <c r="L6" s="18" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="18">
+        <v>3</v>
+      </c>
+      <c r="B7" s="18">
+        <v>2</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="H7" s="19">
+        <v>5</v>
+      </c>
+      <c r="I7" s="17"/>
+      <c r="J7" s="18">
+        <v>6</v>
+      </c>
+      <c r="K7" s="20">
+        <v>44604</v>
+      </c>
+      <c r="L7" s="18" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="18">
+        <v>4</v>
+      </c>
+      <c r="B8" s="18">
+        <v>1</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="18">
+        <v>7</v>
+      </c>
+      <c r="K8" s="20">
+        <v>44611</v>
+      </c>
+      <c r="L8" s="18" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="18">
+        <v>4</v>
+      </c>
+      <c r="B9" s="18">
+        <v>2</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="18">
+        <v>8</v>
+      </c>
+      <c r="K9" s="20">
+        <v>44618</v>
+      </c>
+      <c r="L9" s="18" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="18">
+        <v>5</v>
+      </c>
+      <c r="B10" s="18">
+        <v>1</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="18">
+        <v>9</v>
+      </c>
+      <c r="K10" s="20">
+        <v>44625</v>
+      </c>
+      <c r="L10" s="18" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="18">
+        <v>5</v>
+      </c>
+      <c r="B11" s="18">
+        <v>2</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="18">
+        <v>6</v>
+      </c>
+      <c r="B12" s="18">
+        <v>1</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="18">
+        <v>6</v>
+      </c>
+      <c r="B13" s="18">
+        <v>2</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="18">
+        <v>7</v>
+      </c>
+      <c r="B14" s="18">
+        <v>1</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="18">
+        <v>7</v>
+      </c>
+      <c r="B15" s="18">
+        <v>2</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="18">
+        <v>8</v>
+      </c>
+      <c r="B16" s="18">
+        <v>1</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="18">
+        <v>8</v>
+      </c>
+      <c r="B17" s="18">
+        <v>2</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="18">
+        <v>9</v>
+      </c>
+      <c r="B18" s="18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="18">
+        <v>9</v>
+      </c>
+      <c r="B19" s="18">
+        <v>2</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="18">
+        <v>9</v>
+      </c>
+      <c r="B20" s="18">
+        <v>3</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>344</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>